<commit_message>
Add missing crown dependency file for test
</commit_message>
<xml_diff>
--- a/cypress/fixtures/Fal1-Files/FAL 1-CrownDependency.xlsx
+++ b/cypress/fixtures/Fal1-Files/FAL 1-CrownDependency.xlsx
@@ -5,10 +5,10 @@
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Homeoffice\NMSW-Main\nmsw-ui\cypress\fixtures\Fal1-Files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jayanthi\OneDrive - Home Office (Digital)\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED80ABB5-0D96-4DCE-A6C6-BADD1D712C84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{AEFFB352-A516-420F-8A7A-8A8179E7805D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="ISO 3-letter country codes" sheetId="2" r:id="rId2"/>
     <sheet name="LOCODES" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191028" refMode="R1C1" iterateCount="0" calcOnSave="0" concurrentCalc="0"/>
+  <calcPr calcId="191028" refMode="R1C1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -2441,10 +2441,10 @@
     <t>Hardware and Textiles</t>
   </si>
   <si>
+    <t>GBDVR</t>
+  </si>
+  <si>
     <t>CD NMSW Test Ship</t>
-  </si>
-  <si>
-    <t>Tester</t>
   </si>
   <si>
     <t>Departure from the UK</t>
@@ -2463,7 +2463,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="h:mm:ss&quot; &quot;AM/PM"/>
   </numFmts>
-  <fonts count="24" x14ac:knownFonts="1">
+  <fonts count="23" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color indexed="8"/>
@@ -2608,17 +2608,10 @@
       <name val="Roboto"/>
     </font>
     <font>
-      <sz val="8"/>
-      <color rgb="FF1D1C1D"/>
+      <sz val="10"/>
+      <color rgb="FF0B0C0C"/>
       <name val="Arial"/>
       <family val="2"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
     </font>
   </fonts>
   <fills count="9">
@@ -3245,7 +3238,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="86">
+  <cellXfs count="85">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3335,6 +3328,9 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -3362,7 +3358,7 @@
     <xf numFmtId="0" fontId="20" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3381,9 +3377,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="20" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="14" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -3493,9 +3486,6 @@
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4692,8 +4682,8 @@
   </sheetPr>
   <dimension ref="A1:P26"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A9" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -4722,7 +4712,7 @@
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="47" t="s">
+      <c r="B2" s="31" t="s">
         <v>557</v>
       </c>
       <c r="C2" s="51"/>
@@ -4734,13 +4724,13 @@
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="39" t="s">
-        <v>555</v>
+      <c r="B3" s="40" t="s">
+        <v>556</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="31">
+      <c r="D3" s="32">
         <v>9999990</v>
       </c>
       <c r="E3" s="13" t="s">
@@ -4754,59 +4744,59 @@
       <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="39" t="s">
-        <v>556</v>
+      <c r="B4" s="40" t="s">
+        <v>551</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="39" t="s">
+      <c r="D4" s="40" t="s">
         <v>118</v>
       </c>
       <c r="E4" s="58"/>
       <c r="F4" s="59"/>
     </row>
-    <row r="5" spans="1:6" ht="270" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" ht="270" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="84" t="s">
-        <v>559</v>
+      <c r="B5" s="40" t="s">
+        <v>555</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="44">
+      <c r="D5" s="45">
         <v>45214</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="F5" s="38">
+      <c r="F5" s="39">
         <v>0.5</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="147.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" ht="147.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="39" t="s">
+      <c r="B6" s="84" t="s">
         <v>558</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="45">
+      <c r="D6" s="46">
         <v>45049</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F6" s="38">
+      <c r="F6" s="39">
         <v>4.1666666666666664E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="184.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" ht="184.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>13</v>
       </c>
@@ -4816,13 +4806,13 @@
       <c r="C7" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D7" s="40" t="s">
+      <c r="D7" s="84" t="s">
         <v>559</v>
       </c>
       <c r="E7" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="F7" s="85" t="s">
+      <c r="F7" s="41" t="s">
         <v>559</v>
       </c>
     </row>
@@ -4836,7 +4826,7 @@
       <c r="C8" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="D8" s="37">
+      <c r="D8" s="38">
         <v>10</v>
       </c>
       <c r="E8" s="54"/>
@@ -4846,13 +4836,13 @@
       <c r="A9" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B9" s="41" t="s">
+      <c r="B9" s="42" t="s">
         <v>551</v>
       </c>
       <c r="C9" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="D9" s="33">
+      <c r="D9" s="34">
         <v>987654321</v>
       </c>
       <c r="E9" s="55"/>
@@ -4862,7 +4852,7 @@
       <c r="A10" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="B10" s="42" t="s">
+      <c r="B10" s="43" t="s">
         <v>118</v>
       </c>
       <c r="C10" s="60"/>
@@ -4874,7 +4864,7 @@
       <c r="A11" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="B11" s="33">
+      <c r="B11" s="34">
         <v>5</v>
       </c>
       <c r="C11" s="62"/>
@@ -4886,7 +4876,7 @@
       <c r="A12" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="B12" s="43" t="s">
+      <c r="B12" s="44" t="s">
         <v>552</v>
       </c>
       <c r="C12" s="62"/>
@@ -4898,7 +4888,7 @@
       <c r="A13" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B13" s="46" t="s">
+      <c r="B13" s="47" t="s">
         <v>554</v>
       </c>
       <c r="C13" s="62"/>
@@ -4910,7 +4900,7 @@
       <c r="A14" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="B14" s="34">
+      <c r="B14" s="35">
         <v>20</v>
       </c>
       <c r="C14" s="62"/>
@@ -4922,7 +4912,7 @@
       <c r="A15" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="B15" s="35">
+      <c r="B15" s="36">
         <v>100</v>
       </c>
       <c r="C15" s="62"/>
@@ -4934,7 +4924,7 @@
       <c r="A16" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="B16" s="32"/>
+      <c r="B16" s="33"/>
       <c r="C16" s="62"/>
       <c r="D16" s="63"/>
       <c r="E16" s="55"/>
@@ -5024,7 +5014,7 @@
       <c r="A25" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="B25" s="36"/>
+      <c r="B25" s="37"/>
       <c r="C25" s="62"/>
       <c r="D25" s="63"/>
       <c r="E25" s="55"/>
@@ -7233,26 +7223,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="18390984-f7d9-4502-80ba-82ec344db5fb">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="629dd2dc-abea-47e8-ba88-82202e3ee8ef" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D364DC965387FD4EAF4833DDCF640F91" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c7401bc8bddc44f3d87e6545050f3282">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="18390984-f7d9-4502-80ba-82ec344db5fb" xmlns:ns3="629dd2dc-abea-47e8-ba88-82202e3ee8ef" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="fc3cb6a02f8baa81433631181c409fee" ns2:_="" ns3:_="">
     <xsd:import namespace="18390984-f7d9-4502-80ba-82ec344db5fb"/>
@@ -7489,26 +7459,27 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5C2A0AF4-2234-45DE-BCD6-060ACA865D30}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="18390984-f7d9-4502-80ba-82ec344db5fb"/>
-    <ds:schemaRef ds:uri="629dd2dc-abea-47e8-ba88-82202e3ee8ef"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3A5056AD-6F82-4433-81E7-2CF7DDF58706}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="18390984-f7d9-4502-80ba-82ec344db5fb">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="629dd2dc-abea-47e8-ba88-82202e3ee8ef" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4A6CC910-0FFF-41DD-A80E-A1312D067115}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -7525,4 +7496,23 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3A5056AD-6F82-4433-81E7-2CF7DDF58706}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5C2A0AF4-2234-45DE-BCD6-060ACA865D30}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="18390984-f7d9-4502-80ba-82ec344db5fb"/>
+    <ds:schemaRef ds:uri="629dd2dc-abea-47e8-ba88-82202e3ee8ef"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Test to verify Isle of Man port considering as crown dependency and handling failed/ pending status for submitted reports
</commit_message>
<xml_diff>
--- a/cypress/fixtures/Fal1-Files/FAL 1-CrownDependency.xlsx
+++ b/cypress/fixtures/Fal1-Files/FAL 1-CrownDependency.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jayanthi\OneDrive - Home Office (Digital)\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Homeoffice\NMSW\nmsw-ui\cypress\fixtures\Fal1-Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AEFFB352-A516-420F-8A7A-8A8179E7805D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A2F9A11-096B-4330-B4E7-1CE19D8275C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="ISO 3-letter country codes" sheetId="2" r:id="rId2"/>
     <sheet name="LOCODES" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191028" refMode="R1C1"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -2450,10 +2450,10 @@
     <t>Departure from the UK</t>
   </si>
   <si>
-    <t>JE STH</t>
-  </si>
-  <si>
     <t>GB DVR</t>
+  </si>
+  <si>
+    <t>IM PEL</t>
   </si>
 </sst>
 </file>
@@ -3377,6 +3377,7 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="14" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -3485,7 +3486,6 @@
     <xf numFmtId="49" fontId="0" fillId="8" borderId="34" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4682,8 +4682,8 @@
   </sheetPr>
   <dimension ref="A1:P26"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A9" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -4699,14 +4699,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="50" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="48" t="s">
+      <c r="A1" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="49"/>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50"/>
-      <c r="E1" s="50"/>
-      <c r="F1" s="50"/>
+      <c r="B1" s="50"/>
+      <c r="C1" s="51"/>
+      <c r="D1" s="51"/>
+      <c r="E1" s="51"/>
+      <c r="F1" s="51"/>
     </row>
     <row r="2" spans="1:6" ht="102" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
@@ -4715,10 +4715,10 @@
       <c r="B2" s="31" t="s">
         <v>557</v>
       </c>
-      <c r="C2" s="51"/>
-      <c r="D2" s="52"/>
-      <c r="E2" s="52"/>
-      <c r="F2" s="53"/>
+      <c r="C2" s="52"/>
+      <c r="D2" s="53"/>
+      <c r="E2" s="53"/>
+      <c r="F2" s="54"/>
     </row>
     <row r="3" spans="1:6" ht="90.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
@@ -4753,8 +4753,8 @@
       <c r="D4" s="40" t="s">
         <v>118</v>
       </c>
-      <c r="E4" s="58"/>
-      <c r="F4" s="59"/>
+      <c r="E4" s="59"/>
+      <c r="F4" s="60"/>
     </row>
     <row r="5" spans="1:6" ht="270" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
@@ -4780,8 +4780,8 @@
       <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="84" t="s">
-        <v>558</v>
+      <c r="B6" s="48" t="s">
+        <v>559</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>11</v>
@@ -4806,14 +4806,14 @@
       <c r="C7" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D7" s="84" t="s">
-        <v>559</v>
+      <c r="D7" s="48" t="s">
+        <v>558</v>
       </c>
       <c r="E7" s="6" t="s">
         <v>15</v>
       </c>
       <c r="F7" s="41" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -4829,8 +4829,8 @@
       <c r="D8" s="38">
         <v>10</v>
       </c>
-      <c r="E8" s="54"/>
-      <c r="F8" s="54"/>
+      <c r="E8" s="55"/>
+      <c r="F8" s="55"/>
     </row>
     <row r="9" spans="1:6" ht="41.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="4" t="s">
@@ -4845,8 +4845,8 @@
       <c r="D9" s="34">
         <v>987654321</v>
       </c>
-      <c r="E9" s="55"/>
-      <c r="F9" s="54"/>
+      <c r="E9" s="56"/>
+      <c r="F9" s="55"/>
     </row>
     <row r="10" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="10" t="s">
@@ -4855,10 +4855,10 @@
       <c r="B10" s="43" t="s">
         <v>118</v>
       </c>
-      <c r="C10" s="60"/>
-      <c r="D10" s="61"/>
-      <c r="E10" s="55"/>
-      <c r="F10" s="54"/>
+      <c r="C10" s="61"/>
+      <c r="D10" s="62"/>
+      <c r="E10" s="56"/>
+      <c r="F10" s="55"/>
     </row>
     <row r="11" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="10" t="s">
@@ -4867,10 +4867,10 @@
       <c r="B11" s="34">
         <v>5</v>
       </c>
-      <c r="C11" s="62"/>
-      <c r="D11" s="63"/>
-      <c r="E11" s="55"/>
-      <c r="F11" s="54"/>
+      <c r="C11" s="63"/>
+      <c r="D11" s="64"/>
+      <c r="E11" s="56"/>
+      <c r="F11" s="55"/>
     </row>
     <row r="12" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="10" t="s">
@@ -4879,10 +4879,10 @@
       <c r="B12" s="44" t="s">
         <v>552</v>
       </c>
-      <c r="C12" s="62"/>
-      <c r="D12" s="63"/>
-      <c r="E12" s="55"/>
-      <c r="F12" s="54"/>
+      <c r="C12" s="63"/>
+      <c r="D12" s="64"/>
+      <c r="E12" s="56"/>
+      <c r="F12" s="55"/>
     </row>
     <row r="13" spans="1:6" ht="128.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
@@ -4891,10 +4891,10 @@
       <c r="B13" s="47" t="s">
         <v>554</v>
       </c>
-      <c r="C13" s="62"/>
-      <c r="D13" s="63"/>
-      <c r="E13" s="55"/>
-      <c r="F13" s="54"/>
+      <c r="C13" s="63"/>
+      <c r="D13" s="64"/>
+      <c r="E13" s="56"/>
+      <c r="F13" s="55"/>
     </row>
     <row r="14" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="12" t="s">
@@ -4903,10 +4903,10 @@
       <c r="B14" s="35">
         <v>20</v>
       </c>
-      <c r="C14" s="62"/>
-      <c r="D14" s="63"/>
-      <c r="E14" s="55"/>
-      <c r="F14" s="54"/>
+      <c r="C14" s="63"/>
+      <c r="D14" s="64"/>
+      <c r="E14" s="56"/>
+      <c r="F14" s="55"/>
     </row>
     <row r="15" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="7" t="s">
@@ -4915,120 +4915,120 @@
       <c r="B15" s="36">
         <v>100</v>
       </c>
-      <c r="C15" s="62"/>
-      <c r="D15" s="63"/>
-      <c r="E15" s="55"/>
-      <c r="F15" s="54"/>
+      <c r="C15" s="63"/>
+      <c r="D15" s="64"/>
+      <c r="E15" s="56"/>
+      <c r="F15" s="55"/>
     </row>
     <row r="16" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="7" t="s">
         <v>26</v>
       </c>
       <c r="B16" s="33"/>
-      <c r="C16" s="62"/>
-      <c r="D16" s="63"/>
-      <c r="E16" s="55"/>
-      <c r="F16" s="54"/>
+      <c r="C16" s="63"/>
+      <c r="D16" s="64"/>
+      <c r="E16" s="56"/>
+      <c r="F16" s="55"/>
     </row>
     <row r="17" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="56" t="s">
+      <c r="A17" s="57" t="s">
         <v>27</v>
       </c>
-      <c r="B17" s="57"/>
-      <c r="C17" s="62"/>
-      <c r="D17" s="63"/>
-      <c r="E17" s="55"/>
-      <c r="F17" s="54"/>
+      <c r="B17" s="58"/>
+      <c r="C17" s="63"/>
+      <c r="D17" s="64"/>
+      <c r="E17" s="56"/>
+      <c r="F17" s="55"/>
     </row>
     <row r="18" spans="1:6" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A18" s="7" t="s">
         <v>28</v>
       </c>
       <c r="B18" s="27"/>
-      <c r="C18" s="62"/>
-      <c r="D18" s="63"/>
-      <c r="E18" s="55"/>
-      <c r="F18" s="54"/>
+      <c r="C18" s="63"/>
+      <c r="D18" s="64"/>
+      <c r="E18" s="56"/>
+      <c r="F18" s="55"/>
     </row>
     <row r="19" spans="1:6" ht="33" x14ac:dyDescent="0.35">
       <c r="A19" s="7" t="s">
         <v>29</v>
       </c>
       <c r="B19" s="27"/>
-      <c r="C19" s="62"/>
-      <c r="D19" s="63"/>
-      <c r="E19" s="55"/>
-      <c r="F19" s="54"/>
+      <c r="C19" s="63"/>
+      <c r="D19" s="64"/>
+      <c r="E19" s="56"/>
+      <c r="F19" s="55"/>
     </row>
     <row r="20" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="7" t="s">
         <v>30</v>
       </c>
       <c r="B20" s="27"/>
-      <c r="C20" s="62"/>
-      <c r="D20" s="63"/>
-      <c r="E20" s="55"/>
-      <c r="F20" s="54"/>
+      <c r="C20" s="63"/>
+      <c r="D20" s="64"/>
+      <c r="E20" s="56"/>
+      <c r="F20" s="55"/>
     </row>
     <row r="21" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="7" t="s">
         <v>31</v>
       </c>
       <c r="B21" s="27"/>
-      <c r="C21" s="62"/>
-      <c r="D21" s="63"/>
-      <c r="E21" s="55"/>
-      <c r="F21" s="54"/>
+      <c r="C21" s="63"/>
+      <c r="D21" s="64"/>
+      <c r="E21" s="56"/>
+      <c r="F21" s="55"/>
     </row>
     <row r="22" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="7" t="s">
         <v>32</v>
       </c>
       <c r="B22" s="27"/>
-      <c r="C22" s="62"/>
-      <c r="D22" s="63"/>
-      <c r="E22" s="55"/>
-      <c r="F22" s="54"/>
+      <c r="C22" s="63"/>
+      <c r="D22" s="64"/>
+      <c r="E22" s="56"/>
+      <c r="F22" s="55"/>
     </row>
     <row r="23" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="7" t="s">
         <v>33</v>
       </c>
       <c r="B23" s="27"/>
-      <c r="C23" s="62"/>
-      <c r="D23" s="63"/>
-      <c r="E23" s="55"/>
-      <c r="F23" s="54"/>
+      <c r="C23" s="63"/>
+      <c r="D23" s="64"/>
+      <c r="E23" s="56"/>
+      <c r="F23" s="55"/>
     </row>
     <row r="24" spans="1:6" ht="17.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="7" t="s">
         <v>34</v>
       </c>
       <c r="B24" s="27"/>
-      <c r="C24" s="62"/>
-      <c r="D24" s="63"/>
-      <c r="E24" s="55"/>
-      <c r="F24" s="54"/>
+      <c r="C24" s="63"/>
+      <c r="D24" s="64"/>
+      <c r="E24" s="56"/>
+      <c r="F24" s="55"/>
     </row>
     <row r="25" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="7" t="s">
         <v>35</v>
       </c>
       <c r="B25" s="37"/>
-      <c r="C25" s="62"/>
-      <c r="D25" s="63"/>
-      <c r="E25" s="55"/>
-      <c r="F25" s="54"/>
+      <c r="C25" s="63"/>
+      <c r="D25" s="64"/>
+      <c r="E25" s="56"/>
+      <c r="F25" s="55"/>
     </row>
     <row r="26" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="11" t="s">
         <v>36</v>
       </c>
       <c r="B26" s="27"/>
-      <c r="C26" s="64"/>
-      <c r="D26" s="65"/>
-      <c r="E26" s="55"/>
-      <c r="F26" s="54"/>
+      <c r="C26" s="65"/>
+      <c r="D26" s="66"/>
+      <c r="E26" s="56"/>
+      <c r="F26" s="55"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -5087,11 +5087,11 @@
       <c r="B1" s="28" t="s">
         <v>38</v>
       </c>
-      <c r="C1" s="69" t="s">
+      <c r="C1" s="70" t="s">
         <v>39</v>
       </c>
-      <c r="D1" s="70"/>
-      <c r="E1" s="71"/>
+      <c r="D1" s="71"/>
+      <c r="E1" s="72"/>
       <c r="F1" s="19"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
@@ -5101,9 +5101,9 @@
       <c r="B2" s="28" t="s">
         <v>41</v>
       </c>
-      <c r="C2" s="72"/>
-      <c r="D2" s="73"/>
-      <c r="E2" s="74"/>
+      <c r="C2" s="73"/>
+      <c r="D2" s="74"/>
+      <c r="E2" s="75"/>
       <c r="F2" s="19"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
@@ -5113,11 +5113,11 @@
       <c r="B3" s="28" t="s">
         <v>43</v>
       </c>
-      <c r="C3" s="66" t="s">
+      <c r="C3" s="67" t="s">
         <v>44</v>
       </c>
-      <c r="D3" s="67"/>
-      <c r="E3" s="68"/>
+      <c r="D3" s="68"/>
+      <c r="E3" s="69"/>
       <c r="F3" s="19"/>
     </row>
     <row r="4" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -5127,11 +5127,11 @@
       <c r="B4" s="28" t="s">
         <v>46</v>
       </c>
-      <c r="C4" s="75" t="s">
+      <c r="C4" s="76" t="s">
         <v>47</v>
       </c>
-      <c r="D4" s="76"/>
-      <c r="E4" s="77"/>
+      <c r="D4" s="77"/>
+      <c r="E4" s="78"/>
       <c r="F4" s="19"/>
     </row>
     <row r="5" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -5141,9 +5141,9 @@
       <c r="B5" s="28" t="s">
         <v>49</v>
       </c>
-      <c r="C5" s="78"/>
-      <c r="D5" s="79"/>
-      <c r="E5" s="80"/>
+      <c r="C5" s="79"/>
+      <c r="D5" s="80"/>
+      <c r="E5" s="81"/>
       <c r="F5" s="19"/>
     </row>
     <row r="6" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -5153,9 +5153,9 @@
       <c r="B6" s="28" t="s">
         <v>51</v>
       </c>
-      <c r="C6" s="81"/>
-      <c r="D6" s="82"/>
-      <c r="E6" s="83"/>
+      <c r="C6" s="82"/>
+      <c r="D6" s="83"/>
+      <c r="E6" s="84"/>
       <c r="F6" s="19"/>
     </row>
     <row r="7" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -7223,6 +7223,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="18390984-f7d9-4502-80ba-82ec344db5fb">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="629dd2dc-abea-47e8-ba88-82202e3ee8ef" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D364DC965387FD4EAF4833DDCF640F91" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c7401bc8bddc44f3d87e6545050f3282">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="18390984-f7d9-4502-80ba-82ec344db5fb" xmlns:ns3="629dd2dc-abea-47e8-ba88-82202e3ee8ef" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="fc3cb6a02f8baa81433631181c409fee" ns2:_="" ns3:_="">
     <xsd:import namespace="18390984-f7d9-4502-80ba-82ec344db5fb"/>
@@ -7459,27 +7479,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5C2A0AF4-2234-45DE-BCD6-060ACA865D30}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="18390984-f7d9-4502-80ba-82ec344db5fb"/>
+    <ds:schemaRef ds:uri="629dd2dc-abea-47e8-ba88-82202e3ee8ef"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="18390984-f7d9-4502-80ba-82ec344db5fb">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="629dd2dc-abea-47e8-ba88-82202e3ee8ef" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3A5056AD-6F82-4433-81E7-2CF7DDF58706}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4A6CC910-0FFF-41DD-A80E-A1312D067115}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -7496,23 +7515,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3A5056AD-6F82-4433-81E7-2CF7DDF58706}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5C2A0AF4-2234-45DE-BCD6-060ACA865D30}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="18390984-f7d9-4502-80ba-82ec344db5fb"/>
-    <ds:schemaRef ds:uri="629dd2dc-abea-47e8-ba88-82202e3ee8ef"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Test sign-in and forgotten password link for unverified emails
</commit_message>
<xml_diff>
--- a/cypress/fixtures/Fal1-Files/FAL 1-CrownDependency.xlsx
+++ b/cypress/fixtures/Fal1-Files/FAL 1-CrownDependency.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jayanthi\OneDrive - Home Office (Digital)\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Homeoffice\NMSW\nmsw-ui\cypress\fixtures\Fal1-Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AEFFB352-A516-420F-8A7A-8A8179E7805D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A2F9A11-096B-4330-B4E7-1CE19D8275C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="ISO 3-letter country codes" sheetId="2" r:id="rId2"/>
     <sheet name="LOCODES" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191028" refMode="R1C1"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -2450,10 +2450,10 @@
     <t>Departure from the UK</t>
   </si>
   <si>
-    <t>JE STH</t>
-  </si>
-  <si>
     <t>GB DVR</t>
+  </si>
+  <si>
+    <t>IM PEL</t>
   </si>
 </sst>
 </file>
@@ -3377,6 +3377,7 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="14" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -3485,7 +3486,6 @@
     <xf numFmtId="49" fontId="0" fillId="8" borderId="34" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4682,8 +4682,8 @@
   </sheetPr>
   <dimension ref="A1:P26"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A9" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -4699,14 +4699,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="50" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="48" t="s">
+      <c r="A1" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="49"/>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50"/>
-      <c r="E1" s="50"/>
-      <c r="F1" s="50"/>
+      <c r="B1" s="50"/>
+      <c r="C1" s="51"/>
+      <c r="D1" s="51"/>
+      <c r="E1" s="51"/>
+      <c r="F1" s="51"/>
     </row>
     <row r="2" spans="1:6" ht="102" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
@@ -4715,10 +4715,10 @@
       <c r="B2" s="31" t="s">
         <v>557</v>
       </c>
-      <c r="C2" s="51"/>
-      <c r="D2" s="52"/>
-      <c r="E2" s="52"/>
-      <c r="F2" s="53"/>
+      <c r="C2" s="52"/>
+      <c r="D2" s="53"/>
+      <c r="E2" s="53"/>
+      <c r="F2" s="54"/>
     </row>
     <row r="3" spans="1:6" ht="90.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
@@ -4753,8 +4753,8 @@
       <c r="D4" s="40" t="s">
         <v>118</v>
       </c>
-      <c r="E4" s="58"/>
-      <c r="F4" s="59"/>
+      <c r="E4" s="59"/>
+      <c r="F4" s="60"/>
     </row>
     <row r="5" spans="1:6" ht="270" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
@@ -4780,8 +4780,8 @@
       <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="84" t="s">
-        <v>558</v>
+      <c r="B6" s="48" t="s">
+        <v>559</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>11</v>
@@ -4806,14 +4806,14 @@
       <c r="C7" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D7" s="84" t="s">
-        <v>559</v>
+      <c r="D7" s="48" t="s">
+        <v>558</v>
       </c>
       <c r="E7" s="6" t="s">
         <v>15</v>
       </c>
       <c r="F7" s="41" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -4829,8 +4829,8 @@
       <c r="D8" s="38">
         <v>10</v>
       </c>
-      <c r="E8" s="54"/>
-      <c r="F8" s="54"/>
+      <c r="E8" s="55"/>
+      <c r="F8" s="55"/>
     </row>
     <row r="9" spans="1:6" ht="41.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="4" t="s">
@@ -4845,8 +4845,8 @@
       <c r="D9" s="34">
         <v>987654321</v>
       </c>
-      <c r="E9" s="55"/>
-      <c r="F9" s="54"/>
+      <c r="E9" s="56"/>
+      <c r="F9" s="55"/>
     </row>
     <row r="10" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="10" t="s">
@@ -4855,10 +4855,10 @@
       <c r="B10" s="43" t="s">
         <v>118</v>
       </c>
-      <c r="C10" s="60"/>
-      <c r="D10" s="61"/>
-      <c r="E10" s="55"/>
-      <c r="F10" s="54"/>
+      <c r="C10" s="61"/>
+      <c r="D10" s="62"/>
+      <c r="E10" s="56"/>
+      <c r="F10" s="55"/>
     </row>
     <row r="11" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="10" t="s">
@@ -4867,10 +4867,10 @@
       <c r="B11" s="34">
         <v>5</v>
       </c>
-      <c r="C11" s="62"/>
-      <c r="D11" s="63"/>
-      <c r="E11" s="55"/>
-      <c r="F11" s="54"/>
+      <c r="C11" s="63"/>
+      <c r="D11" s="64"/>
+      <c r="E11" s="56"/>
+      <c r="F11" s="55"/>
     </row>
     <row r="12" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="10" t="s">
@@ -4879,10 +4879,10 @@
       <c r="B12" s="44" t="s">
         <v>552</v>
       </c>
-      <c r="C12" s="62"/>
-      <c r="D12" s="63"/>
-      <c r="E12" s="55"/>
-      <c r="F12" s="54"/>
+      <c r="C12" s="63"/>
+      <c r="D12" s="64"/>
+      <c r="E12" s="56"/>
+      <c r="F12" s="55"/>
     </row>
     <row r="13" spans="1:6" ht="128.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
@@ -4891,10 +4891,10 @@
       <c r="B13" s="47" t="s">
         <v>554</v>
       </c>
-      <c r="C13" s="62"/>
-      <c r="D13" s="63"/>
-      <c r="E13" s="55"/>
-      <c r="F13" s="54"/>
+      <c r="C13" s="63"/>
+      <c r="D13" s="64"/>
+      <c r="E13" s="56"/>
+      <c r="F13" s="55"/>
     </row>
     <row r="14" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="12" t="s">
@@ -4903,10 +4903,10 @@
       <c r="B14" s="35">
         <v>20</v>
       </c>
-      <c r="C14" s="62"/>
-      <c r="D14" s="63"/>
-      <c r="E14" s="55"/>
-      <c r="F14" s="54"/>
+      <c r="C14" s="63"/>
+      <c r="D14" s="64"/>
+      <c r="E14" s="56"/>
+      <c r="F14" s="55"/>
     </row>
     <row r="15" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="7" t="s">
@@ -4915,120 +4915,120 @@
       <c r="B15" s="36">
         <v>100</v>
       </c>
-      <c r="C15" s="62"/>
-      <c r="D15" s="63"/>
-      <c r="E15" s="55"/>
-      <c r="F15" s="54"/>
+      <c r="C15" s="63"/>
+      <c r="D15" s="64"/>
+      <c r="E15" s="56"/>
+      <c r="F15" s="55"/>
     </row>
     <row r="16" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="7" t="s">
         <v>26</v>
       </c>
       <c r="B16" s="33"/>
-      <c r="C16" s="62"/>
-      <c r="D16" s="63"/>
-      <c r="E16" s="55"/>
-      <c r="F16" s="54"/>
+      <c r="C16" s="63"/>
+      <c r="D16" s="64"/>
+      <c r="E16" s="56"/>
+      <c r="F16" s="55"/>
     </row>
     <row r="17" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="56" t="s">
+      <c r="A17" s="57" t="s">
         <v>27</v>
       </c>
-      <c r="B17" s="57"/>
-      <c r="C17" s="62"/>
-      <c r="D17" s="63"/>
-      <c r="E17" s="55"/>
-      <c r="F17" s="54"/>
+      <c r="B17" s="58"/>
+      <c r="C17" s="63"/>
+      <c r="D17" s="64"/>
+      <c r="E17" s="56"/>
+      <c r="F17" s="55"/>
     </row>
     <row r="18" spans="1:6" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A18" s="7" t="s">
         <v>28</v>
       </c>
       <c r="B18" s="27"/>
-      <c r="C18" s="62"/>
-      <c r="D18" s="63"/>
-      <c r="E18" s="55"/>
-      <c r="F18" s="54"/>
+      <c r="C18" s="63"/>
+      <c r="D18" s="64"/>
+      <c r="E18" s="56"/>
+      <c r="F18" s="55"/>
     </row>
     <row r="19" spans="1:6" ht="33" x14ac:dyDescent="0.35">
       <c r="A19" s="7" t="s">
         <v>29</v>
       </c>
       <c r="B19" s="27"/>
-      <c r="C19" s="62"/>
-      <c r="D19" s="63"/>
-      <c r="E19" s="55"/>
-      <c r="F19" s="54"/>
+      <c r="C19" s="63"/>
+      <c r="D19" s="64"/>
+      <c r="E19" s="56"/>
+      <c r="F19" s="55"/>
     </row>
     <row r="20" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="7" t="s">
         <v>30</v>
       </c>
       <c r="B20" s="27"/>
-      <c r="C20" s="62"/>
-      <c r="D20" s="63"/>
-      <c r="E20" s="55"/>
-      <c r="F20" s="54"/>
+      <c r="C20" s="63"/>
+      <c r="D20" s="64"/>
+      <c r="E20" s="56"/>
+      <c r="F20" s="55"/>
     </row>
     <row r="21" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="7" t="s">
         <v>31</v>
       </c>
       <c r="B21" s="27"/>
-      <c r="C21" s="62"/>
-      <c r="D21" s="63"/>
-      <c r="E21" s="55"/>
-      <c r="F21" s="54"/>
+      <c r="C21" s="63"/>
+      <c r="D21" s="64"/>
+      <c r="E21" s="56"/>
+      <c r="F21" s="55"/>
     </row>
     <row r="22" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="7" t="s">
         <v>32</v>
       </c>
       <c r="B22" s="27"/>
-      <c r="C22" s="62"/>
-      <c r="D22" s="63"/>
-      <c r="E22" s="55"/>
-      <c r="F22" s="54"/>
+      <c r="C22" s="63"/>
+      <c r="D22" s="64"/>
+      <c r="E22" s="56"/>
+      <c r="F22" s="55"/>
     </row>
     <row r="23" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="7" t="s">
         <v>33</v>
       </c>
       <c r="B23" s="27"/>
-      <c r="C23" s="62"/>
-      <c r="D23" s="63"/>
-      <c r="E23" s="55"/>
-      <c r="F23" s="54"/>
+      <c r="C23" s="63"/>
+      <c r="D23" s="64"/>
+      <c r="E23" s="56"/>
+      <c r="F23" s="55"/>
     </row>
     <row r="24" spans="1:6" ht="17.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="7" t="s">
         <v>34</v>
       </c>
       <c r="B24" s="27"/>
-      <c r="C24" s="62"/>
-      <c r="D24" s="63"/>
-      <c r="E24" s="55"/>
-      <c r="F24" s="54"/>
+      <c r="C24" s="63"/>
+      <c r="D24" s="64"/>
+      <c r="E24" s="56"/>
+      <c r="F24" s="55"/>
     </row>
     <row r="25" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="7" t="s">
         <v>35</v>
       </c>
       <c r="B25" s="37"/>
-      <c r="C25" s="62"/>
-      <c r="D25" s="63"/>
-      <c r="E25" s="55"/>
-      <c r="F25" s="54"/>
+      <c r="C25" s="63"/>
+      <c r="D25" s="64"/>
+      <c r="E25" s="56"/>
+      <c r="F25" s="55"/>
     </row>
     <row r="26" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="11" t="s">
         <v>36</v>
       </c>
       <c r="B26" s="27"/>
-      <c r="C26" s="64"/>
-      <c r="D26" s="65"/>
-      <c r="E26" s="55"/>
-      <c r="F26" s="54"/>
+      <c r="C26" s="65"/>
+      <c r="D26" s="66"/>
+      <c r="E26" s="56"/>
+      <c r="F26" s="55"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -5087,11 +5087,11 @@
       <c r="B1" s="28" t="s">
         <v>38</v>
       </c>
-      <c r="C1" s="69" t="s">
+      <c r="C1" s="70" t="s">
         <v>39</v>
       </c>
-      <c r="D1" s="70"/>
-      <c r="E1" s="71"/>
+      <c r="D1" s="71"/>
+      <c r="E1" s="72"/>
       <c r="F1" s="19"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
@@ -5101,9 +5101,9 @@
       <c r="B2" s="28" t="s">
         <v>41</v>
       </c>
-      <c r="C2" s="72"/>
-      <c r="D2" s="73"/>
-      <c r="E2" s="74"/>
+      <c r="C2" s="73"/>
+      <c r="D2" s="74"/>
+      <c r="E2" s="75"/>
       <c r="F2" s="19"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
@@ -5113,11 +5113,11 @@
       <c r="B3" s="28" t="s">
         <v>43</v>
       </c>
-      <c r="C3" s="66" t="s">
+      <c r="C3" s="67" t="s">
         <v>44</v>
       </c>
-      <c r="D3" s="67"/>
-      <c r="E3" s="68"/>
+      <c r="D3" s="68"/>
+      <c r="E3" s="69"/>
       <c r="F3" s="19"/>
     </row>
     <row r="4" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -5127,11 +5127,11 @@
       <c r="B4" s="28" t="s">
         <v>46</v>
       </c>
-      <c r="C4" s="75" t="s">
+      <c r="C4" s="76" t="s">
         <v>47</v>
       </c>
-      <c r="D4" s="76"/>
-      <c r="E4" s="77"/>
+      <c r="D4" s="77"/>
+      <c r="E4" s="78"/>
       <c r="F4" s="19"/>
     </row>
     <row r="5" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -5141,9 +5141,9 @@
       <c r="B5" s="28" t="s">
         <v>49</v>
       </c>
-      <c r="C5" s="78"/>
-      <c r="D5" s="79"/>
-      <c r="E5" s="80"/>
+      <c r="C5" s="79"/>
+      <c r="D5" s="80"/>
+      <c r="E5" s="81"/>
       <c r="F5" s="19"/>
     </row>
     <row r="6" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -5153,9 +5153,9 @@
       <c r="B6" s="28" t="s">
         <v>51</v>
       </c>
-      <c r="C6" s="81"/>
-      <c r="D6" s="82"/>
-      <c r="E6" s="83"/>
+      <c r="C6" s="82"/>
+      <c r="D6" s="83"/>
+      <c r="E6" s="84"/>
       <c r="F6" s="19"/>
     </row>
     <row r="7" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -7223,6 +7223,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="18390984-f7d9-4502-80ba-82ec344db5fb">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="629dd2dc-abea-47e8-ba88-82202e3ee8ef" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D364DC965387FD4EAF4833DDCF640F91" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c7401bc8bddc44f3d87e6545050f3282">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="18390984-f7d9-4502-80ba-82ec344db5fb" xmlns:ns3="629dd2dc-abea-47e8-ba88-82202e3ee8ef" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="fc3cb6a02f8baa81433631181c409fee" ns2:_="" ns3:_="">
     <xsd:import namespace="18390984-f7d9-4502-80ba-82ec344db5fb"/>
@@ -7459,27 +7479,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5C2A0AF4-2234-45DE-BCD6-060ACA865D30}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="18390984-f7d9-4502-80ba-82ec344db5fb"/>
+    <ds:schemaRef ds:uri="629dd2dc-abea-47e8-ba88-82202e3ee8ef"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="18390984-f7d9-4502-80ba-82ec344db5fb">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="629dd2dc-abea-47e8-ba88-82202e3ee8ef" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3A5056AD-6F82-4433-81E7-2CF7DDF58706}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4A6CC910-0FFF-41DD-A80E-A1312D067115}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -7496,23 +7515,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3A5056AD-6F82-4433-81E7-2CF7DDF58706}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5C2A0AF4-2234-45DE-BCD6-060ACA865D30}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="18390984-f7d9-4502-80ba-82ec344db5fb"/>
-    <ds:schemaRef ds:uri="629dd2dc-abea-47e8-ba88-82202e3ee8ef"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>